<commit_message>
update readme, fix test bug
</commit_message>
<xml_diff>
--- a/tests/test-data.xlsx
+++ b/tests/test-data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">SKU</t>
+  </si>
   <si>
     <t xml:space="preserve">Quantity Available</t>
   </si>
@@ -49,7 +52,25 @@
     <t xml:space="preserve">70030_200-4XL</t>
   </si>
   <si>
-    <t xml:space="preserve">70115_990-L</t>
+    <t xml:space="preserve">70123_410-XS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70123_410-S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70123_410-M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70123_410-L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70123_410-XL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70123_410-2XL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70123_410-3XL</t>
   </si>
 </sst>
 </file>
@@ -84,7 +105,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,7 +170,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -160,10 +180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="230" zoomScaleNormal="230" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,22 +192,24 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>38</v>
@@ -195,39 +217,39 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>104</v>
@@ -235,7 +257,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>48</v>
@@ -243,10 +265,58 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>1</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>